<commit_message>
contenidos cargados bien en excel
</commit_message>
<xml_diff>
--- a/BernardoRivero.xlsx
+++ b/BernardoRivero.xlsx
@@ -549,7 +549,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A Ad,</t>
+          <t xml:space="preserve"> A, Ad</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fi Hx,</t>
+          <t xml:space="preserve"> Fi</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> H H, Hd,</t>
+          <t xml:space="preserve"> H, Hd</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">

</xml_diff>

<commit_message>
contenidos y determinantes cargados bien
</commit_message>
<xml_diff>
--- a/BernardoRivero.xlsx
+++ b/BernardoRivero.xlsx
@@ -594,7 +594,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> m, C</t>
+          <t xml:space="preserve"> C, m</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> M, M</t>
+          <t xml:space="preserve"> M</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">

</xml_diff>